<commit_message>
Revised Prepare.supply to handle cst hubs and terminals
</commit_message>
<xml_diff>
--- a/scenarios/01_original_data/cst_schedule.xlsx
+++ b/scenarios/01_original_data/cst_schedule.xlsx
@@ -63,9 +63,6 @@
     <t>Aufenthaltsdauer</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>Strecke</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Gland</t>
+  </si>
+  <si>
+    <t>CST</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E5" sqref="E5"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,29 +658,29 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
       <c r="H1" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
       <c r="K1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
@@ -718,10 +718,10 @@
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="21">
         <v>1</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="21">
         <v>2</v>
@@ -839,24 +839,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1">
-      <UserInfo>
-        <DisplayName>Fiechter Stefan (G-VB-KV)</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58121ac2-18af-4ecc-8c57-48116ccff2c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008677C648B6E3F447A1E688F51092B38F" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="451330d46dcb5de4eb40eb8723282060">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="58121ac2-18af-4ecc-8c57-48116ccff2c8" xmlns:ns3="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a2226fc1a7392e01a1c3c16b3944abb" ns2:_="" ns3:_="">
     <xsd:import namespace="58121ac2-18af-4ecc-8c57-48116ccff2c8"/>
@@ -1099,7 +1081,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1108,24 +1090,25 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCDD99EF-EC37-452A-831C-2A7706A6F0AF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1"/>
-    <ds:schemaRef ds:uri="58121ac2-18af-4ecc-8c57-48116ccff2c8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1">
+      <UserInfo>
+        <DisplayName>Fiechter Stefan (G-VB-KV)</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58121ac2-18af-4ecc-8c57-48116ccff2c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D035154E-F094-4019-A80D-294BB662C7F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1144,10 +1127,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{333AE5A3-2EC6-4FD6-B87F-1B4185EFD233}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCDD99EF-EC37-452A-831C-2A7706A6F0AF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e189a8ff-9db3-4f77-a12f-1afe0dbec0d1"/>
+    <ds:schemaRef ds:uri="58121ac2-18af-4ecc-8c57-48116ccff2c8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>